<commit_message>
Major & Minor words replaced
by Functional & Non-Functional respectively. Some clerical mistakes corrected.
</commit_message>
<xml_diff>
--- a/Support/Quality Assurance/CHKL_ADTPEG.xlsx
+++ b/Support/Quality Assurance/CHKL_ADTPEG.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15255" windowHeight="8445"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="15255" windowHeight="8445" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Revision History" sheetId="1" r:id="rId1"/>
@@ -50,9 +50,6 @@
     <t>Measurement and Analysis related activity</t>
   </si>
   <si>
-    <t>Has the MBR been prepared? (Have all the Measurement data viz Validation Defect Detection Percentage, Review Effectiveness, Schedule Variance, Effort Variance and Training Effectiveness been gathered from all the projects during the measurement periods?)</t>
-  </si>
-  <si>
     <t>Are all the inputs being received from process practitioners/ PPQA/Training Group/Metrics Reports being analyzed by PEG?</t>
   </si>
   <si>
@@ -114,14 +111,17 @@
     <t>Genus Innovation Limited</t>
   </si>
   <si>
-    <t>Template Version - 1</t>
+    <t>Template Version - 2</t>
+  </si>
+  <si>
+    <t>Has the MBR been prepared? (Have all the Measurement data viz Line Rejection Percentage, Schedule Variance, and Training Effectiveness been gathered from all the projects during the measurement periods?)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,7 +286,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -323,6 +323,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Accent1" xfId="3" builtinId="31"/>
@@ -398,7 +399,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -549,6 +550,11 @@
       <tableStyleElement type="firstColumnStripe" dxfId="8"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -640,6 +646,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -674,6 +681,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -849,76 +857,76 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.5">
+    <row r="1" spans="1:5" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="22.5">
+    <row r="5" spans="1:5" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -931,14 +939,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" customWidth="1"/>
     <col min="2" max="2" width="90.140625" customWidth="1"/>
@@ -946,28 +954,28 @@
     <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" s="5" customFormat="1" ht="22.5">
+    <row r="2" spans="1:4" s="5" customFormat="1" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="20.25" thickBot="1">
+    <row r="5" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="21" thickTop="1" thickBot="1">
+    <row r="6" spans="1:4" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="21" thickTop="1" thickBot="1">
+    <row r="7" spans="1:4" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" thickTop="1"/>
-    <row r="9" spans="1:4" ht="60">
+    <row r="8" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>3</v>
       </c>
@@ -975,133 +983,133 @@
         <v>4</v>
       </c>
       <c r="C9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="30">
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>1</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="10"/>
+        <v>11</v>
+      </c>
+      <c r="C10" s="24"/>
       <c r="D10" s="10"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>2</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="10"/>
+        <v>12</v>
+      </c>
+      <c r="C11" s="24"/>
       <c r="D11" s="10"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>3</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="10"/>
+        <v>13</v>
+      </c>
+      <c r="C12" s="24"/>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>4</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="C13" s="24"/>
       <c r="D13" s="10"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>5</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="10"/>
+        <v>15</v>
+      </c>
+      <c r="C14" s="24"/>
       <c r="D14" s="10"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>6</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="10"/>
+        <v>16</v>
+      </c>
+      <c r="C15" s="24"/>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>7</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="10"/>
+      <c r="C16" s="24"/>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>8</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="10"/>
+        <v>17</v>
+      </c>
+      <c r="C17" s="24"/>
       <c r="D17" s="10"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <v>9</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="12"/>
+        <v>18</v>
+      </c>
+      <c r="C18" s="24"/>
       <c r="D18" s="12"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>10</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="10"/>
+      <c r="C19" s="24"/>
       <c r="D19" s="10"/>
     </row>
-    <row r="20" spans="1:4" s="18" customFormat="1">
+    <row r="20" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>11</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="10"/>
+        <v>27</v>
+      </c>
+      <c r="C20" s="24"/>
       <c r="D20" s="10"/>
     </row>
-    <row r="21" spans="1:4" ht="30">
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>12</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="10"/>
+        <v>28</v>
+      </c>
+      <c r="C21" s="24"/>
       <c r="D21" s="10"/>
     </row>
-    <row r="22" spans="1:4" s="4" customFormat="1">
+    <row r="22" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="B22" s="14" t="s">
         <v>10</v>
@@ -1109,108 +1117,111 @@
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
     </row>
-    <row r="23" spans="1:4" ht="45">
+    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>1</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="10"/>
+        <v>32</v>
+      </c>
+      <c r="C23" s="24"/>
       <c r="D23" s="10"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>2</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="10"/>
+      <c r="C24" s="24"/>
       <c r="D24" s="10"/>
     </row>
-    <row r="25" spans="1:4" s="21" customFormat="1">
+    <row r="25" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>3</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="10"/>
+        <v>29</v>
+      </c>
+      <c r="C25" s="24"/>
       <c r="D25" s="10"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>4</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="10"/>
+      <c r="C26" s="24"/>
       <c r="D26" s="10"/>
     </row>
-    <row r="27" spans="1:4" s="4" customFormat="1">
+    <row r="27" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>1</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C28" s="10"/>
+        <v>21</v>
+      </c>
+      <c r="C28" s="24"/>
       <c r="D28" s="10"/>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>2</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" s="10"/>
+        <v>22</v>
+      </c>
+      <c r="C29" s="24"/>
       <c r="D29" s="10"/>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>3</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30" s="10"/>
+        <v>23</v>
+      </c>
+      <c r="C30" s="24"/>
       <c r="D30" s="10"/>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>4</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C31" s="10"/>
+        <v>24</v>
+      </c>
+      <c r="C31" s="24"/>
       <c r="D31" s="10"/>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="16">
         <v>5</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="17"/>
+        <v>25</v>
+      </c>
+      <c r="C32" s="24"/>
       <c r="D32" s="17"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10:C21 C23:C27">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C27">
       <formula1>"Conformance,Major Non-Conformance,Minor Non-Conformance,Observation, NA"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10:C21 C23:C26 C28:C32">
+      <formula1>"Conformance,Functional Non-Conformance,Non Functional Non-Conformance,Observation, NA"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>